<commit_message>
Update of static Excels
</commit_message>
<xml_diff>
--- a/private/INDIVIDUAL_LOCALIZATIONS_UI_7.xlsx
+++ b/private/INDIVIDUAL_LOCALIZATIONS_UI_7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6283F8E7-EAF5-4437-AF4C-D996248C5A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4B1D2A-69E0-49CE-BCD5-34BB4C8F9A2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7545" yWindow="1740" windowWidth="22245" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="1965" windowWidth="22245" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTL" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12033" uniqueCount="7293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12048" uniqueCount="7306">
   <si>
     <t>en_US</t>
   </si>
@@ -21917,6 +21917,45 @@
   </si>
   <si>
     <t>Na mesz na patchu {patch} {platform} {gameId} | lolvvv</t>
+  </si>
+  <si>
+    <t>label|montage</t>
+  </si>
+  <si>
+    <t>Montage</t>
+  </si>
+  <si>
+    <t>Montaje</t>
+  </si>
+  <si>
+    <t>Montagem</t>
+  </si>
+  <si>
+    <t>Montaż</t>
+  </si>
+  <si>
+    <t>モンタージュ</t>
+  </si>
+  <si>
+    <t>蒙太奇</t>
+  </si>
+  <si>
+    <t>Montaggio</t>
+  </si>
+  <si>
+    <t>Монтаж</t>
+  </si>
+  <si>
+    <t>몽타주</t>
+  </si>
+  <si>
+    <t>Montaj</t>
+  </si>
+  <si>
+    <t>Dựng phim</t>
+  </si>
+  <si>
+    <t>A compilation of many clips</t>
   </si>
 </sst>
 </file>
@@ -22368,11 +22407,11 @@
   <sheetPr codeName="Tabelle1">
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB602"/>
+  <dimension ref="A1:AB603"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z91" sqref="Z91"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -22386,10 +22425,10 @@
     <col min="7" max="7" width="27.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="52.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="44.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="54.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="49.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="52.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="44.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="54.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="49.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="41.85546875" style="1" customWidth="1"/>
     <col min="15" max="15" width="46" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.42578125" style="1" customWidth="1"/>
@@ -49541,7 +49580,7 @@
         <v>6916</v>
       </c>
     </row>
-    <row r="593" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="593" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F593" s="26" t="s">
         <v>6223</v>
       </c>
@@ -49562,7 +49601,7 @@
         <v>6917</v>
       </c>
     </row>
-    <row r="594" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="594" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F594" s="26" t="s">
         <v>6224</v>
       </c>
@@ -49583,7 +49622,7 @@
         <v>6918</v>
       </c>
     </row>
-    <row r="595" spans="6:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="595" spans="6:28" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F595" s="31" t="s">
         <v>6231</v>
       </c>
@@ -49615,7 +49654,7 @@
         <v>6919</v>
       </c>
     </row>
-    <row r="596" spans="6:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="6:28" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F596" s="31" t="s">
         <v>6235</v>
       </c>
@@ -49637,7 +49676,7 @@
         <v>6920</v>
       </c>
     </row>
-    <row r="597" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="597" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F597" s="3" t="s">
         <v>6500</v>
       </c>
@@ -49654,7 +49693,7 @@
         <v>6921</v>
       </c>
     </row>
-    <row r="598" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="598" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F598" s="26" t="s">
         <v>6501</v>
       </c>
@@ -49671,7 +49710,7 @@
         <v>6922</v>
       </c>
     </row>
-    <row r="599" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="599" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F599" s="26" t="s">
         <v>6502</v>
       </c>
@@ -49688,7 +49727,7 @@
         <v>6923</v>
       </c>
     </row>
-    <row r="600" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="600" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F600" s="26" t="s">
         <v>6503</v>
       </c>
@@ -49705,7 +49744,7 @@
         <v>6924</v>
       </c>
     </row>
-    <row r="601" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="601" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F601" s="26" t="s">
         <v>6504</v>
       </c>
@@ -49722,7 +49761,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="602" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="602" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F602" s="3" t="s">
         <v>6937</v>
       </c>
@@ -49752,6 +49791,53 @@
       </c>
       <c r="Z602" s="27" t="s">
         <v>6946</v>
+      </c>
+    </row>
+    <row r="603" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F603" s="3" t="s">
+        <v>7293</v>
+      </c>
+      <c r="G603" s="4" t="s">
+        <v>7305</v>
+      </c>
+      <c r="I603" s="24" t="s">
+        <v>7294</v>
+      </c>
+      <c r="J603" s="24" t="s">
+        <v>7294</v>
+      </c>
+      <c r="M603" s="27" t="s">
+        <v>7295</v>
+      </c>
+      <c r="N603" s="24" t="s">
+        <v>7294</v>
+      </c>
+      <c r="Q603" s="27" t="s">
+        <v>7300</v>
+      </c>
+      <c r="R603" s="1" t="s">
+        <v>7298</v>
+      </c>
+      <c r="S603" s="27" t="s">
+        <v>7302</v>
+      </c>
+      <c r="U603" s="24" t="s">
+        <v>7297</v>
+      </c>
+      <c r="V603" s="27" t="s">
+        <v>7296</v>
+      </c>
+      <c r="X603" s="1" t="s">
+        <v>7301</v>
+      </c>
+      <c r="Z603" s="24" t="s">
+        <v>7303</v>
+      </c>
+      <c r="AA603" s="24" t="s">
+        <v>7304</v>
+      </c>
+      <c r="AB603" s="1" t="s">
+        <v>7299</v>
       </c>
     </row>
   </sheetData>
@@ -49794,10 +49880,10 @@
   <dimension ref="A1:S230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P187" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S2" sqref="S2:S230"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
german runes loc added
</commit_message>
<xml_diff>
--- a/private/INDIVIDUAL_LOCALIZATIONS_UI_7.xlsx
+++ b/private/INDIVIDUAL_LOCALIZATIONS_UI_7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ABD9D9-0EA0-4EED-8622-8CAE9B6D0861}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7862F9-8CD8-4186-B028-113AD42E3AFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20040" yWindow="210" windowWidth="27825" windowHeight="20100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="255" windowWidth="27825" windowHeight="20100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTL" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12301" uniqueCount="7789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12369" uniqueCount="7857">
   <si>
     <t>en_US</t>
   </si>
@@ -23022,9 +23022,6 @@
     <t>Unsealed Spellbook</t>
   </si>
   <si>
-    <t>This keystone rune slows enemy champion by your first basic attack. This slow can by followed up by a skill shot of {championName} to force the opponent in a dangerous situation.</t>
-  </si>
-  <si>
     <t>GlacialAugment</t>
   </si>
   <si>
@@ -23235,9 +23232,6 @@
     <t>Ingenious Hunter</t>
   </si>
   <si>
-    <t>{RavenousHunter} is the final rune on the {Domination} tree. This rune gives some sustain during skirmishes and small damage trades. The additional health is nothing to scoff at and can mean the difference between winning or losing a trade.</t>
-  </si>
-  <si>
     <t>RavenousHunter</t>
   </si>
   <si>
@@ -23295,9 +23289,6 @@
     <t>Cheap Shot</t>
   </si>
   <si>
-    <t>This keystone rune helps you to win short trades in your lane by increasing your attackspeed at the beginning of a skirmish.</t>
-  </si>
-  <si>
     <t>HailOfBlades</t>
   </si>
   <si>
@@ -23331,9 +23322,6 @@
     <t>Last Stand</t>
   </si>
   <si>
-    <t>If the enemy team consists of multiple tanks, then {CutDown} is the best rune choice.</t>
-  </si>
-  <si>
     <t>CutDown</t>
   </si>
   <si>
@@ -23412,9 +23400,6 @@
     <t>Fleet Footwork</t>
   </si>
   <si>
-    <t>It gives {championName} a nice head start in team fights and allows to put out more damage in that time window.</t>
-  </si>
-  <si>
     <t>LethalTempo</t>
   </si>
   <si>
@@ -23433,10 +23418,230 @@
     <t>Type</t>
   </si>
   <si>
-    <t>{SuddenImpact} increases your damage after using a dash or being invisible. This is due to how easy it is to use on {championName} with the amount of ways he has to dash, blink or stealth. The additional lethality helps to take down the priority targets that much easier.</t>
-  </si>
-  <si>
     <t>{TimeWarpTonic} gives you additional sustain by boosting your {Item2003} and {Item2010}.</t>
+  </si>
+  <si>
+    <t>{RavenousHunter} is the final rune on the {Domination} tree. This rune gives some survivability during short fights and damage trades during the laning phase. The additional health is nothing to scoff at and can mean the difference between winning or losing a battle.</t>
+  </si>
+  <si>
+    <t>This keystone rune helps you to win short trades in your lane by increasing your attackspeed at the beginning of a fight.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune generiert Ihnen eine Menge Sustain und erhöht Ihre Überlebensfähigkeit gegen Poke-Champions in der Lane.</t>
+  </si>
+  <si>
+    <t>{Overheal} wandelt Heilung, die über die maximale Gesundheit von {championName} hinausgeht, in einen Schild um, der zusätzliche Sicherheit und Tankiness bietet.</t>
+  </si>
+  <si>
+    <t>{PresenceOfMind} hilft {championName} bei Manaproblemen, indem es Mana wiederherstellt und den maximalen Manapool von {championName} erhöht.</t>
+  </si>
+  <si>
+    <t>{RavenousHunter} ist die letzte Rune auf dem {Domination} Baum. Diese Rune verleiht etwas Überlebensfähigkeit während kurzer Kämpfe und Schadenstrades in der Laning-Phase. Die zusätzlichen Lebenspunkte sind nicht zu verachten und können den Unterschied zwischen Sieg oder Niederlage in einem Kampf ausmachen.</t>
+  </si>
+  <si>
+    <t>{MagicalFootwear} ermöglicht es Spielern, sich auf die wesentlichen Kerngegenstände zu konzentrieren, ohne die zusätzlichen 300 Gold für Stiefel ausgeben zu müssen.</t>
+  </si>
+  <si>
+    <t>Du kannst Schulden machen, um Gegenstände zu kaufen, was als negatives Gold in Deiner Schatzkammer angezeigt wird. Eine kleine Leihgebühr wird auf den Goldbetrag, den Du nach Verlassen des Ladens schulden, aufgeschlagen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{MinionDematerializer} hilft Ihnen, die Phase der Minion-Welle zu kontrollieren. </t>
+  </si>
+  <si>
+    <t>{BiscuitDelivery} ist eine großartige Rune für das Laning, da sie sowohl Gesundheit als auch Mana erhält, was in aggressiveren Lanes helfen kann.</t>
+  </si>
+  <si>
+    <t>{CosmicInsight} gewährt Beschwörerzauber- und Gegenstands-Eile.</t>
+  </si>
+  <si>
+    <t>{championName} kann diese Rune sehr leicht mit Grundangriffen aktivieren, was gut mit der Schadenserhöhung von {PressTheAttack} synergiert, sobald diese aktiviert ist.</t>
+  </si>
+  <si>
+    <t>{Triumph} stellt auf {championName} einen Teil der fehlenden Gesundheit wieder her und gewährt Bonusgold, wenn ein Champion getötet wird.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{LegendAlacrity} gewährt {championName} zusätzliches Angriffstempo. </t>
+  </si>
+  <si>
+    <t>{championName} erhält zusätzliche Zähigkeit mit jedem Stapel von {LegendTenacity}.</t>
+  </si>
+  <si>
+    <t>{championName} verursacht mit {CoupDeGrace} mehr Schaden an Zielen mit niedriger Gesundheit.</t>
+  </si>
+  <si>
+    <t>{PhaseRush} bietet mehr Flexibilität und Optionen, um in und aus der Gefahr zu weben, was hilfreich sein kann, da dies im Wesentlichen der Haupt-Spielstil von {championName} ist.</t>
+  </si>
+  <si>
+    <t>{Waterwalking} gewährt Bewegungstempo im Fluss, was {championName} hilft, sich schneller auf der Karte zu bewegen. Der zusätzliche Schaden hilft auch in den so wichtigen Drachen- und Baronkämpfen.</t>
+  </si>
+  <si>
+    <t>{Knochenpanzerung} macht {championName} insgesamt tanker, indem es die Menge an Poke-Schaden im frühen Spiel vermindert.</t>
+  </si>
+  <si>
+    <t>{Präzision} verbessert den Angriffs- und Dauerschaden von {championName} während des gesamten Matches.</t>
+  </si>
+  <si>
+    <t>Beherrschung} verbessert den Burst-Schaden und die Attentatswerkzeuge von {championName}.</t>
+  </si>
+  <si>
+    <t>{Sorcery} stärkt die Fähigkeiten von {championName} und erhöht die verfügbaren Champion-Ressourcen.</t>
+  </si>
+  <si>
+    <t>{Resolve} stärkt die Haltbarkeit von {championName} und erhöht die Tankiness.</t>
+  </si>
+  <si>
+    <t>{Inspiration} eröffnet {championName} im Laufe des Matches kreative Möglichkeiten.</t>
+  </si>
+  <si>
+    <t>This keystone rune gives {championName} a nice head start in team fights and allows to put out more damage in that time window.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune verschafft {ChampionName} einen schönen Vorsprung in Teamkämpfen und ermöglicht es, in diesem Zeitfenster mehr Schaden zu verursachen.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune sorgt für zusätzliche Power in den späteren Phasen eines Spiels. Sobald {Conqueror} vollständig gestapelt ist, verursacht {championName} zusätzlichen Schaden und erhält Lebenserhaltung.</t>
+  </si>
+  <si>
+    <t>{LegendBloodline} gibt Lebensraub, was später beim Gewinnen von Trades und Kämpfen hilft.</t>
+  </si>
+  <si>
+    <t>If the enemy team consists of multiple tanks, then the rune {CutDown} is the best choice.</t>
+  </si>
+  <si>
+    <t>Wenn das gegnerische Team aus mehreren Tanks besteht, dann ist die Rune {CutDown} die beste Wahl.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune sorgt für Burst-Schaden und hilft Dir dabei, die gegnerischen Carrys niederzustrecken.</t>
+  </si>
+  <si>
+    <t>Mit {LastStand} teilst Du mehr Schaden aus, während Du bei niedriger Gesundheit bist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobald Du Stiefel kaufst, kannst Du die aktive Fähigkeit von {Predator} verwenden. Nach einer kurzen Wirkzeit erhält {championName} einen Bonus an Bewegungsgeschwindigkeit, während er sich auf gegnerische Champions zubewegt. </t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune ist perfekt für Roaming und Ganking.
+Diese Keystone-Rune verleiht Dir während des gesamten Matches zusätzlichen Schaden.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune hilft Dir, kurze Trades in Deiner Lane zu gewinnen, indem sie Dein Angriffstempo zu Beginn eines Kampfes erhöht.</t>
+  </si>
+  <si>
+    <t>{CheapShot} sorgt dafür, dass Du Gegnern mit eingeschränkter Bewegung mehr Schaden zufügen, was eine großartige Synergie mit dem Setup von {championName} darstellt.</t>
+  </si>
+  <si>
+    <t>{TasteOfBlood} heilt {championName}, sobald Du einem gegnerischen Champion Schaden zufügst.</t>
+  </si>
+  <si>
+    <t>{SuddenImpact} increases your damage after dashing or being invisible. This is due to how easy it is to use on {championName} with the amount of ways he has to dash, blink or stealth. The additional lethality helps to take down the priority targets that much easier.</t>
+  </si>
+  <si>
+    <t>{ZombieWard} hilft Dir, Deine Sicht auf der Karte zu erweitern. Die Sicht ist in LoL sehr wirkungsvoll und hilft Dir, unnötige Tode zu vermeiden.</t>
+  </si>
+  <si>
+    <t>{SuddenImpact} erhöht Deinen Schaden, nachdem Du gesprungen bist oder unsichtbar warst. Das liegt daran, dass es bei {championName} so einfach zu verwenden ist, da der Champion so viele Möglichkeiten hat, zu flitzen, zu blinken oder sich zu tarnen. Die zusätzliche Tödlichkeit hilft dabei, die vorrangigen Ziele viel leichter auszuschalten.</t>
+  </si>
+  <si>
+    <t>{GhostPoro} hilft Dir, Deine Sicht für einen längeren Zeitraum auf der Karte zu behalten. Vision ist in LoL sehr wirkungsvoll und hilft Dir, unnötige Tode zu vermeiden.</t>
+  </si>
+  <si>
+    <t>{EyeballCollection} ist als nächstes dran. Diese gewährt dem Anwender zusätzlichen Schaden mit jeder Tötung, die er erzielt.</t>
+  </si>
+  <si>
+    <t>{IngeniousHunter} gibt Dir bei jeder einzigartigen Champion-Tötung Gegenstands-Eile.</t>
+  </si>
+  <si>
+    <t>{RelentlessHunter} erhöht Deine Bewegungsgeschwindigkeit außerhalb des Kampfes bei jeder einzigartigen Champion-Tötung.</t>
+  </si>
+  <si>
+    <t>{UltimateHunter} erhöht bei jeder einzigartigen Champion-Tötung die ultimative Eile von {championName}.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune fügt Deinen Fähigkeiten mehr Poke-Schaden zu. Und gewährt zusätzlich einen zusätzlichen Schild, wenn {championName} einen Verbündeten mit Fähigkeiten befähigt oder schützt.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune fügt Deinen Fähigkeiten mehr Schaden zu und erhöht Ihre Kraft in der Laning-Phase.</t>
+  </si>
+  <si>
+    <t>{NullifyingOrb} gewährt Dir einen Schild, sobald {championName} durch magischen Schaden in Mitleidenschaft gezogen wird. Diese Rune wird Dir sehr helfen, gegen Fähigkeitsstärke-Champions mit viel Burst zu überleben.</t>
+  </si>
+  <si>
+    <t>Im Anschluss daran nimmst Du normalerweise {ManaflowBand} für zusätzliches Mana und Mana-Sustain.</t>
+  </si>
+  <si>
+    <t>{Transcendence} für etwas mehr Fähigkeits-Eile.</t>
+  </si>
+  <si>
+    <t>{NimbusCloak}, der beim Wirken eines Beschwörerzaubers Bewegungstempo gewährt, funktioniert insbesondere bei Junglern erstaunlich gut, da sie den Beschwörerzauber mit der kürzesten Abklingzeit, {SummonerSmite}, nehmen.</t>
+  </si>
+  <si>
+    <t>{Celerity} erhöht alle Boni auf die Bewegungsgeschwindigkeit von {championName}.</t>
+  </si>
+  <si>
+    <t>{AbsoluteFocus} gewährt zusätzlichen Schaden, solange {championName} noch nicht volle Gesundheit hat.</t>
+  </si>
+  <si>
+    <t>{Scorch} erhöht Deine frühe Spielkontrolle.</t>
+  </si>
+  <si>
+    <t>{GatheringStorm} erhöht Deine Late-Game-Versicherung.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune gibt {championName} viel Sustain und hilft, Deinen gegnerischen Champion aus der Lane zu drängen.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune stärkt Dich und erhöht sowohl Deine Rüstung als auch Deine Magieresistenz, wenn Sie einen Champion bewegungsunfähig machen. {AfterShock} synergiert sowohl mit der schieren Menge an Crowd Control, die {championName} besitzt, als auch mit der Notwendigkeit, tanky zu sein, sobald Du angreifst.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune gewährt Deinem Teamkollegen und Dir selbst einen Schild, sobald einer von Euch durch einen gegnerischen Champion Schaden erleidet.</t>
+  </si>
+  <si>
+    <t>{Demolish} erhöht Deinen Druck auf die gegnerischen Türme. Diese Keystone-Rune hilft Dir, schlechte Roams oder Backtimings Deines Lane-Gegners zu bestrafen.</t>
+  </si>
+  <si>
+    <t>{FontOfLife} versorgt Deinen Botlaner mit mehr Sustain, indem es ihn immer dann heilt, wenn er einen Champion angreift, dessen Bewegung Du gerade beeinträchtigt hast.</t>
+  </si>
+  <si>
+    <t>{ShieldBash} steigert Deine Tankfähigkeit und stärkt Deinen nächsten Basisangriff, während Du abgeschirmt bist.</t>
+  </si>
+  <si>
+    <t>{Conditioning} erhöht die Tankfähigkeit von {championName} nach der Laning-Phase.</t>
+  </si>
+  <si>
+    <t>{SecondWind} erhöht Ihre Durchhaltefähigkeit in der Lane durch Heilung, nachdem Du von einem gegnerischen Champion Schaden genommen haben.</t>
+  </si>
+  <si>
+    <t>{Overgrowth} erhöht Deine maximalen Lebenspunktezahl.</t>
+  </si>
+  <si>
+    <t>{Revitalize} erhöht die Heilungen und Schilde, die Du wirkst oder erhältst.</t>
+  </si>
+  <si>
+    <t>{Unflinching} erhöht die Zähigkeit von {championName} basierend auf Deiner fehlenden Gesundheit.</t>
+  </si>
+  <si>
+    <t>This keystone rune slows enemy champion on your first basic attack. This slow can by followed up by a skill shot of {championName} to force the opponent in a dangerous situation.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune verlangsamt den gegnerischen Champion bei Deinem ersten Grundangriff. Diese Verlangsamung kann durch einen Fertigkeitshieb von {ChampionName} fortgesetzt werden, um den Gegner in eine gefährliche Situation zu zwingen.</t>
+  </si>
+  <si>
+    <t>Mit dieser Keystone-Rune kannst Du einen Beschwörerzauber für den einmaligen Gebrauch erstellen. Der neue Beschwörerzauber ersetzt einen Deiner aktuellen Beschwörerzauber und bleibt verfügbar, bis er verwendet oder ersetzt wird. {UnsealedSpellbook} hat einige einzigartige Regeln, die besagen, dass ein bestimmter Beschwörerzauber nicht wieder ausgewählt werden kann, bis drei andere einzigartige Zauber genommen wurden. LoL-Profispieler werden {UnsealedSpellbook} oft verwenden, um sich in ihrer aktuellen oder bevorstehenden Situation zu helfen. Stehst Du kurz davor, den letzten Drachen für einen Seelen-Buff zu bekämpfen? Dank {UnsealedSpellbook} kann {championName} {SummonerSmite} aufheben, um seinem Jungler zu helfen, den Drachen für das Team zu sichern. Es gibt zahllose Umstände, unter denen ein bestimmter Beschwörerzauber das Spiel auf den Kopf stellen kann, und genau hier glänzt {UnsealedSpellbook} am meisten.</t>
+  </si>
+  <si>
+    <t>Diese Keystone-Rune gewährt in regelmäßigen Abständen eine einmalige Verwendung einer anderen zufälligen Keystone-Rune. Nachdem Du die gegebene Keystone-Rune nicht verwendet hast, wird eine weitere zufällige Keystone-Rune gewährt, während Du nicht im Kampf bist. Beim Betreten des Spawn-Punktes wird die aktuelle Keystone-Rune neu gewürfelt. Viele unterschiedliche Keystone-Runen passen zum Setup von {championName}, deshalb ist {MasterKey} eine gute Wahl.</t>
+  </si>
+  <si>
+    <t>Wenn Du eine zusätzliche Möglichkeit hast, die Lücke mit der {HextechFlashtraption} zu schließen, wird ein Angriff viel einfacher durchzuführen sein.</t>
+  </si>
+  <si>
+    <t>Du erhälst kostenlos einen {Item2423}, der einen Überraschungsmoment für Dein gegnerisches Team auslösen kann.</t>
+  </si>
+  <si>
+    <t>{championName} erhält durch {ApproachVelocity} zusätzliches Bewegungstempo, während er sich auf gegnerische Champions zubewegt, die bewegungsunfähig oder verlangsamt sind. Diese Rune ist perfekt, um Angriffen Deiner Teamkameraden zu folgen.</t>
+  </si>
+  <si>
+    <t>{TimeWarpTonic} gibt Dir zusätzliche Unterstützung, indem sie Deinen {Item2003} und {Item2010} verstärkt.</t>
   </si>
 </sst>
 </file>
@@ -64426,8 +64631,8 @@
   <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64445,16 +64650,16 @@
         <v>7605</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>7786</v>
+        <v>7781</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>618</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>7785</v>
+        <v>7780</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>7784</v>
+        <v>7779</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>0</v>
@@ -64517,7 +64722,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7613</v>
       </c>
@@ -64528,16 +64733,19 @@
         <v>7346</v>
       </c>
       <c r="D2" t="s">
-        <v>7783</v>
+        <v>7778</v>
       </c>
       <c r="E2">
         <v>8005</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>7782</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+        <v>7777</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>7794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7613</v>
       </c>
@@ -64548,16 +64756,19 @@
         <v>7349</v>
       </c>
       <c r="D3" t="s">
-        <v>7781</v>
+        <v>7776</v>
       </c>
       <c r="E3">
         <v>8008</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>7780</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+        <v>7807</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>7808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7613</v>
       </c>
@@ -64565,19 +64776,22 @@
         <v>7646</v>
       </c>
       <c r="C4" t="s">
-        <v>7779</v>
+        <v>7775</v>
       </c>
       <c r="D4" t="s">
-        <v>7778</v>
+        <v>7774</v>
       </c>
       <c r="E4">
         <v>8021</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>7777</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+        <v>7773</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>7785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7613</v>
       </c>
@@ -64585,19 +64799,22 @@
         <v>7646</v>
       </c>
       <c r="C5" t="s">
-        <v>7776</v>
+        <v>7772</v>
       </c>
       <c r="D5" t="s">
-        <v>7776</v>
+        <v>7772</v>
       </c>
       <c r="E5">
         <v>8010</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>7775</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+        <v>7771</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>7809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7613</v>
       </c>
@@ -64605,19 +64822,22 @@
         <v>7636</v>
       </c>
       <c r="C6" t="s">
-        <v>7774</v>
+        <v>7770</v>
       </c>
       <c r="D6" t="s">
-        <v>7774</v>
+        <v>7770</v>
       </c>
       <c r="E6">
         <v>9101</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>7773</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+        <v>7769</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>7786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7613</v>
       </c>
@@ -64625,19 +64845,22 @@
         <v>7636</v>
       </c>
       <c r="C7" t="s">
-        <v>7772</v>
+        <v>7768</v>
       </c>
       <c r="D7" t="s">
-        <v>7772</v>
+        <v>7768</v>
       </c>
       <c r="E7">
         <v>9111</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>7771</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+        <v>7767</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>7795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7613</v>
       </c>
@@ -64645,19 +64868,22 @@
         <v>7636</v>
       </c>
       <c r="C8" t="s">
-        <v>7770</v>
+        <v>7766</v>
       </c>
       <c r="D8" t="s">
-        <v>7769</v>
+        <v>7765</v>
       </c>
       <c r="E8">
         <v>8009</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>7768</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+        <v>7764</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>7787</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7613</v>
       </c>
@@ -64665,19 +64891,22 @@
         <v>7626</v>
       </c>
       <c r="C9" t="s">
-        <v>7767</v>
+        <v>7763</v>
       </c>
       <c r="D9" t="s">
-        <v>7766</v>
+        <v>7762</v>
       </c>
       <c r="E9">
         <v>9104</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>7765</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+        <v>7761</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>7796</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7613</v>
       </c>
@@ -64685,19 +64914,22 @@
         <v>7626</v>
       </c>
       <c r="C10" t="s">
-        <v>7764</v>
+        <v>7760</v>
       </c>
       <c r="D10" t="s">
-        <v>7763</v>
+        <v>7759</v>
       </c>
       <c r="E10">
         <v>9105</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>7762</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+        <v>7758</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>7797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7613</v>
       </c>
@@ -64705,16 +64937,19 @@
         <v>7626</v>
       </c>
       <c r="C11" t="s">
-        <v>7761</v>
+        <v>7757</v>
       </c>
       <c r="D11" t="s">
-        <v>7760</v>
+        <v>7756</v>
       </c>
       <c r="E11">
         <v>9103</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>7759</v>
+        <v>7755</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>7810</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -64725,16 +64960,19 @@
         <v>7616</v>
       </c>
       <c r="C12" t="s">
-        <v>7758</v>
+        <v>7754</v>
       </c>
       <c r="D12" t="s">
-        <v>7757</v>
+        <v>7753</v>
       </c>
       <c r="E12">
         <v>8014</v>
       </c>
       <c r="F12" s="42" t="s">
-        <v>7756</v>
+        <v>7752</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>7798</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -64745,19 +64983,22 @@
         <v>7616</v>
       </c>
       <c r="C13" t="s">
-        <v>7755</v>
+        <v>7751</v>
       </c>
       <c r="D13" t="s">
-        <v>7754</v>
+        <v>7750</v>
       </c>
       <c r="E13">
         <v>8017</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>7753</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+        <v>7811</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>7812</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7613</v>
       </c>
@@ -64765,16 +65006,19 @@
         <v>7616</v>
       </c>
       <c r="C14" t="s">
-        <v>7752</v>
+        <v>7749</v>
       </c>
       <c r="D14" t="s">
-        <v>7751</v>
+        <v>7748</v>
       </c>
       <c r="E14">
         <v>8299</v>
       </c>
       <c r="F14" s="42" t="s">
-        <v>7750</v>
+        <v>7747</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>7814</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -64794,10 +65038,13 @@
         <v>8112</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>7749</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+        <v>7746</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>7813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7611</v>
       </c>
@@ -64805,19 +65052,22 @@
         <v>7646</v>
       </c>
       <c r="C16" t="s">
-        <v>7748</v>
+        <v>7745</v>
       </c>
       <c r="D16" t="s">
-        <v>7748</v>
+        <v>7745</v>
       </c>
       <c r="E16">
         <v>8124</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>7747</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7744</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>7815</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7611</v>
       </c>
@@ -64825,19 +65075,22 @@
         <v>7646</v>
       </c>
       <c r="C17" t="s">
-        <v>7746</v>
+        <v>7743</v>
       </c>
       <c r="D17" t="s">
-        <v>7745</v>
+        <v>7742</v>
       </c>
       <c r="E17">
         <v>8128</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>7744</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>7741</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>7816</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7611</v>
       </c>
@@ -64845,19 +65098,22 @@
         <v>7646</v>
       </c>
       <c r="C18" t="s">
-        <v>7743</v>
+        <v>7740</v>
       </c>
       <c r="D18" t="s">
-        <v>7742</v>
+        <v>7739</v>
       </c>
       <c r="E18">
         <v>9923</v>
       </c>
       <c r="F18" s="42" t="s">
-        <v>7741</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>7784</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>7817</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7611</v>
       </c>
@@ -64865,18 +65121,20 @@
         <v>7636</v>
       </c>
       <c r="C19" t="s">
-        <v>7740</v>
+        <v>7738</v>
       </c>
       <c r="D19" t="s">
-        <v>7739</v>
+        <v>7737</v>
       </c>
       <c r="E19">
         <v>8126</v>
       </c>
       <c r="F19" s="44" t="s">
-        <v>7738</v>
-      </c>
-      <c r="G19" s="44"/>
+        <v>7736</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>7818</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -64886,19 +65144,22 @@
         <v>7636</v>
       </c>
       <c r="C20" t="s">
-        <v>7737</v>
+        <v>7735</v>
       </c>
       <c r="D20" t="s">
-        <v>7736</v>
+        <v>7734</v>
       </c>
       <c r="E20">
         <v>8139</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>7735</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>7733</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>7819</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7611</v>
       </c>
@@ -64906,19 +65167,22 @@
         <v>7636</v>
       </c>
       <c r="C21" t="s">
-        <v>7734</v>
+        <v>7732</v>
       </c>
       <c r="D21" t="s">
-        <v>7733</v>
+        <v>7731</v>
       </c>
       <c r="E21">
         <v>8143</v>
       </c>
       <c r="F21" s="44" t="s">
-        <v>7787</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>7820</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>7822</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7611</v>
       </c>
@@ -64926,19 +65190,22 @@
         <v>7626</v>
       </c>
       <c r="C22" t="s">
-        <v>7732</v>
+        <v>7730</v>
       </c>
       <c r="D22" t="s">
-        <v>7731</v>
+        <v>7729</v>
       </c>
       <c r="E22">
         <v>8136</v>
       </c>
       <c r="F22" s="42" t="s">
-        <v>7730</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>7728</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>7821</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7611</v>
       </c>
@@ -64946,19 +65213,22 @@
         <v>7626</v>
       </c>
       <c r="C23" t="s">
-        <v>7729</v>
+        <v>7727</v>
       </c>
       <c r="D23" t="s">
-        <v>7728</v>
+        <v>7726</v>
       </c>
       <c r="E23">
         <v>8120</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>7727</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>7725</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>7823</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7611</v>
       </c>
@@ -64966,19 +65236,22 @@
         <v>7626</v>
       </c>
       <c r="C24" t="s">
-        <v>7726</v>
+        <v>7724</v>
       </c>
       <c r="D24" t="s">
-        <v>7725</v>
+        <v>7723</v>
       </c>
       <c r="E24">
         <v>8138</v>
       </c>
       <c r="F24" s="44" t="s">
-        <v>7724</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>7722</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>7824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7611</v>
       </c>
@@ -64986,19 +65259,22 @@
         <v>7616</v>
       </c>
       <c r="C25" t="s">
-        <v>7723</v>
+        <v>7721</v>
       </c>
       <c r="D25" t="s">
-        <v>7722</v>
+        <v>7720</v>
       </c>
       <c r="E25">
         <v>8135</v>
       </c>
       <c r="F25" s="44" t="s">
-        <v>7721</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7783</v>
+      </c>
+      <c r="G25" s="41" t="s">
+        <v>7788</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7611</v>
       </c>
@@ -65006,19 +65282,22 @@
         <v>7616</v>
       </c>
       <c r="C26" t="s">
-        <v>7720</v>
+        <v>7719</v>
       </c>
       <c r="D26" t="s">
-        <v>7719</v>
+        <v>7718</v>
       </c>
       <c r="E26">
         <v>8134</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>7718</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>7717</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>7825</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7611</v>
       </c>
@@ -65026,18 +65305,20 @@
         <v>7616</v>
       </c>
       <c r="C27" t="s">
-        <v>7717</v>
+        <v>7716</v>
       </c>
       <c r="D27" t="s">
-        <v>7716</v>
+        <v>7715</v>
       </c>
       <c r="E27">
         <v>8105</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>7715</v>
-      </c>
-      <c r="G27" s="44"/>
+        <v>7714</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>7826</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -65047,19 +65328,22 @@
         <v>7616</v>
       </c>
       <c r="C28" t="s">
-        <v>7714</v>
+        <v>7713</v>
       </c>
       <c r="D28" t="s">
-        <v>7713</v>
+        <v>7712</v>
       </c>
       <c r="E28">
         <v>8106</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>7712</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>7711</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>7827</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7609</v>
       </c>
@@ -65067,16 +65351,19 @@
         <v>7646</v>
       </c>
       <c r="C29" t="s">
-        <v>7711</v>
+        <v>7710</v>
       </c>
       <c r="D29" t="s">
-        <v>7710</v>
+        <v>7709</v>
       </c>
       <c r="E29">
         <v>8214</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>7709</v>
+        <v>7708</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>7828</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -65087,19 +65374,22 @@
         <v>7646</v>
       </c>
       <c r="C30" t="s">
-        <v>7708</v>
+        <v>7707</v>
       </c>
       <c r="D30" t="s">
-        <v>7707</v>
+        <v>7706</v>
       </c>
       <c r="E30">
         <v>8229</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>7706</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>7705</v>
+      </c>
+      <c r="G30" s="41" t="s">
+        <v>7829</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7609</v>
       </c>
@@ -65110,16 +65400,19 @@
         <v>7303</v>
       </c>
       <c r="D31" t="s">
-        <v>7705</v>
+        <v>7704</v>
       </c>
       <c r="E31">
         <v>8230</v>
       </c>
       <c r="F31" s="44" t="s">
-        <v>7704</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>7703</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>7799</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7609</v>
       </c>
@@ -65127,19 +65420,22 @@
         <v>7636</v>
       </c>
       <c r="C32" t="s">
-        <v>7703</v>
+        <v>7702</v>
       </c>
       <c r="D32" t="s">
-        <v>7702</v>
+        <v>7701</v>
       </c>
       <c r="E32">
         <v>8224</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>7701</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7700</v>
+      </c>
+      <c r="G32" s="41" t="s">
+        <v>7830</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7609</v>
       </c>
@@ -65147,19 +65443,22 @@
         <v>7636</v>
       </c>
       <c r="C33" t="s">
-        <v>7700</v>
+        <v>7699</v>
       </c>
       <c r="D33" t="s">
-        <v>7699</v>
+        <v>7698</v>
       </c>
       <c r="E33">
         <v>8226</v>
       </c>
       <c r="F33" s="44" t="s">
-        <v>7698</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>7697</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>7831</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7609</v>
       </c>
@@ -65167,19 +65466,22 @@
         <v>7636</v>
       </c>
       <c r="C34" t="s">
-        <v>7697</v>
+        <v>7696</v>
       </c>
       <c r="D34" t="s">
-        <v>7696</v>
+        <v>7695</v>
       </c>
       <c r="E34">
         <v>8275</v>
       </c>
       <c r="F34" s="44" t="s">
-        <v>7695</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7694</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>7833</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7609</v>
       </c>
@@ -65187,19 +65489,22 @@
         <v>7626</v>
       </c>
       <c r="C35" t="s">
-        <v>7694</v>
+        <v>7693</v>
       </c>
       <c r="D35" t="s">
-        <v>7694</v>
+        <v>7693</v>
       </c>
       <c r="E35">
         <v>8210</v>
       </c>
       <c r="F35" s="44" t="s">
-        <v>7693</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7692</v>
+      </c>
+      <c r="G35" s="41" t="s">
+        <v>7832</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7609</v>
       </c>
@@ -65207,19 +65512,22 @@
         <v>7626</v>
       </c>
       <c r="C36" t="s">
-        <v>7692</v>
+        <v>7691</v>
       </c>
       <c r="D36" t="s">
-        <v>7692</v>
+        <v>7691</v>
       </c>
       <c r="E36">
         <v>8234</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>7691</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7690</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>7834</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7609</v>
       </c>
@@ -65227,19 +65535,22 @@
         <v>7626</v>
       </c>
       <c r="C37" t="s">
-        <v>7690</v>
+        <v>7689</v>
       </c>
       <c r="D37" t="s">
-        <v>7689</v>
+        <v>7688</v>
       </c>
       <c r="E37">
         <v>8233</v>
       </c>
       <c r="F37" s="42" t="s">
-        <v>7688</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7687</v>
+      </c>
+      <c r="G37" s="41" t="s">
+        <v>7835</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7609</v>
       </c>
@@ -65247,19 +65558,22 @@
         <v>7616</v>
       </c>
       <c r="C38" t="s">
-        <v>7687</v>
+        <v>7686</v>
       </c>
       <c r="D38" t="s">
-        <v>7687</v>
+        <v>7686</v>
       </c>
       <c r="E38">
         <v>8237</v>
       </c>
       <c r="F38" s="44" t="s">
-        <v>7686</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>7685</v>
+      </c>
+      <c r="G38" s="41" t="s">
+        <v>7836</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7609</v>
       </c>
@@ -65267,19 +65581,22 @@
         <v>7616</v>
       </c>
       <c r="C39" t="s">
-        <v>7685</v>
+        <v>7684</v>
       </c>
       <c r="D39" t="s">
-        <v>7685</v>
+        <v>7684</v>
       </c>
       <c r="E39">
         <v>8232</v>
       </c>
       <c r="F39" s="44" t="s">
-        <v>7684</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7683</v>
+      </c>
+      <c r="G39" s="41" t="s">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7609</v>
       </c>
@@ -65287,19 +65604,22 @@
         <v>7616</v>
       </c>
       <c r="C40" t="s">
-        <v>7683</v>
+        <v>7682</v>
       </c>
       <c r="D40" t="s">
-        <v>7682</v>
+        <v>7681</v>
       </c>
       <c r="E40">
         <v>8236</v>
       </c>
       <c r="F40" s="44" t="s">
-        <v>7681</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7680</v>
+      </c>
+      <c r="G40" s="41" t="s">
+        <v>7837</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6050</v>
       </c>
@@ -65307,19 +65627,22 @@
         <v>7646</v>
       </c>
       <c r="C41" t="s">
-        <v>7680</v>
+        <v>7679</v>
       </c>
       <c r="D41" t="s">
-        <v>7679</v>
+        <v>7678</v>
       </c>
       <c r="E41">
         <v>8437</v>
       </c>
       <c r="F41" s="42" t="s">
-        <v>7678</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>7677</v>
+      </c>
+      <c r="G41" s="41" t="s">
+        <v>7838</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6050</v>
       </c>
@@ -65336,10 +65659,13 @@
         <v>8439</v>
       </c>
       <c r="F42" s="44" t="s">
-        <v>7677</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7676</v>
+      </c>
+      <c r="G42" s="41" t="s">
+        <v>7839</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6050</v>
       </c>
@@ -65347,19 +65673,22 @@
         <v>7646</v>
       </c>
       <c r="C43" t="s">
-        <v>7676</v>
+        <v>7675</v>
       </c>
       <c r="D43" t="s">
-        <v>7676</v>
+        <v>7675</v>
       </c>
       <c r="E43">
         <v>8465</v>
       </c>
       <c r="F43" s="42" t="s">
-        <v>7675</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7674</v>
+      </c>
+      <c r="G43" s="41" t="s">
+        <v>7840</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6050</v>
       </c>
@@ -65367,19 +65696,22 @@
         <v>7636</v>
       </c>
       <c r="C44" t="s">
-        <v>7674</v>
+        <v>7673</v>
       </c>
       <c r="D44" t="s">
-        <v>7674</v>
+        <v>7673</v>
       </c>
       <c r="E44">
         <v>8446</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>7673</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7672</v>
+      </c>
+      <c r="G44" s="41" t="s">
+        <v>7841</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6050</v>
       </c>
@@ -65387,19 +65719,22 @@
         <v>7636</v>
       </c>
       <c r="C45" t="s">
-        <v>7672</v>
+        <v>7671</v>
       </c>
       <c r="D45" t="s">
-        <v>7671</v>
+        <v>7670</v>
       </c>
       <c r="E45">
         <v>8463</v>
       </c>
       <c r="F45" s="44" t="s">
-        <v>7670</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7669</v>
+      </c>
+      <c r="G45" s="41" t="s">
+        <v>7842</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>6050</v>
       </c>
@@ -65407,19 +65742,22 @@
         <v>7636</v>
       </c>
       <c r="C46" t="s">
-        <v>7669</v>
+        <v>7668</v>
       </c>
       <c r="D46" t="s">
-        <v>7668</v>
+        <v>7667</v>
       </c>
       <c r="E46">
         <v>8401</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>7667</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7666</v>
+      </c>
+      <c r="G46" s="41" t="s">
+        <v>7843</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6050</v>
       </c>
@@ -65427,19 +65765,22 @@
         <v>7626</v>
       </c>
       <c r="C47" t="s">
-        <v>7666</v>
+        <v>7665</v>
       </c>
       <c r="D47" t="s">
-        <v>7666</v>
+        <v>7665</v>
       </c>
       <c r="E47">
         <v>8429</v>
       </c>
       <c r="F47" s="42" t="s">
-        <v>7665</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7664</v>
+      </c>
+      <c r="G47" s="41" t="s">
+        <v>7844</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6050</v>
       </c>
@@ -65447,19 +65788,22 @@
         <v>7626</v>
       </c>
       <c r="C48" t="s">
-        <v>7664</v>
+        <v>7663</v>
       </c>
       <c r="D48" t="s">
-        <v>7663</v>
+        <v>7662</v>
       </c>
       <c r="E48">
         <v>8444</v>
       </c>
       <c r="F48" s="42" t="s">
-        <v>7662</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>7661</v>
+      </c>
+      <c r="G48" s="41" t="s">
+        <v>7845</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6050</v>
       </c>
@@ -65467,16 +65811,19 @@
         <v>7626</v>
       </c>
       <c r="C49" t="s">
-        <v>7661</v>
+        <v>7660</v>
       </c>
       <c r="D49" t="s">
-        <v>7660</v>
+        <v>7659</v>
       </c>
       <c r="E49">
         <v>8473</v>
       </c>
       <c r="F49" s="44" t="s">
-        <v>7659</v>
+        <v>7658</v>
+      </c>
+      <c r="G49" s="41" t="s">
+        <v>7801</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -65487,19 +65834,22 @@
         <v>7616</v>
       </c>
       <c r="C50" t="s">
-        <v>7658</v>
+        <v>7657</v>
       </c>
       <c r="D50" t="s">
-        <v>7658</v>
+        <v>7657</v>
       </c>
       <c r="E50">
         <v>8451</v>
       </c>
       <c r="F50" s="44" t="s">
-        <v>7657</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7656</v>
+      </c>
+      <c r="G50" s="41" t="s">
+        <v>7846</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6050</v>
       </c>
@@ -65507,19 +65857,22 @@
         <v>7616</v>
       </c>
       <c r="C51" t="s">
-        <v>7656</v>
+        <v>7655</v>
       </c>
       <c r="D51" t="s">
-        <v>7656</v>
+        <v>7655</v>
       </c>
       <c r="E51">
         <v>8453</v>
       </c>
       <c r="F51" s="42" t="s">
-        <v>7655</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7654</v>
+      </c>
+      <c r="G51" s="41" t="s">
+        <v>7847</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6050</v>
       </c>
@@ -65527,19 +65880,22 @@
         <v>7616</v>
       </c>
       <c r="C52" t="s">
-        <v>7654</v>
+        <v>7653</v>
       </c>
       <c r="D52" t="s">
-        <v>7654</v>
+        <v>7653</v>
       </c>
       <c r="E52">
         <v>8242</v>
       </c>
       <c r="F52" s="42" t="s">
-        <v>7653</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>7652</v>
+      </c>
+      <c r="G52" s="41" t="s">
+        <v>7848</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7606</v>
       </c>
@@ -65547,19 +65903,22 @@
         <v>7646</v>
       </c>
       <c r="C53" t="s">
-        <v>7652</v>
+        <v>7651</v>
       </c>
       <c r="D53" t="s">
-        <v>7651</v>
+        <v>7650</v>
       </c>
       <c r="E53">
         <v>8351</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>7650</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+        <v>7849</v>
+      </c>
+      <c r="G53" s="41" t="s">
+        <v>7850</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7606</v>
       </c>
@@ -65578,8 +65937,11 @@
       <c r="F54" s="44" t="s">
         <v>7647</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G54" s="41" t="s">
+        <v>7851</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>7606</v>
       </c>
@@ -65598,8 +65960,11 @@
       <c r="F55" s="42" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G55" s="41" t="s">
+        <v>7852</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7606</v>
       </c>
@@ -65618,9 +65983,11 @@
       <c r="F56" s="42" t="s">
         <v>7640</v>
       </c>
-      <c r="G56" s="44"/>
-    </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G56" s="44" t="s">
+        <v>7853</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7606</v>
       </c>
@@ -65639,9 +66006,11 @@
       <c r="F57" s="44" t="s">
         <v>7637</v>
       </c>
-      <c r="G57" s="44"/>
-    </row>
-    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G57" s="44" t="s">
+        <v>7789</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>7606</v>
       </c>
@@ -65660,8 +66029,11 @@
       <c r="F58" s="42" t="s">
         <v>7633</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G58" s="41" t="s">
+        <v>7854</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7606</v>
       </c>
@@ -65680,8 +66052,11 @@
       <c r="F59" s="42" t="s">
         <v>7630</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="41" t="s">
+        <v>7790</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>7606</v>
       </c>
@@ -65700,8 +66075,11 @@
       <c r="F60" s="42" t="s">
         <v>7627</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G60" s="41" t="s">
+        <v>7791</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7606</v>
       </c>
@@ -65720,9 +66098,11 @@
       <c r="F61" s="44" t="s">
         <v>7623</v>
       </c>
-      <c r="G61" s="44"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G61" s="44" t="s">
+        <v>7792</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7606</v>
       </c>
@@ -65741,9 +66121,11 @@
       <c r="F62" s="44" t="s">
         <v>7620</v>
       </c>
-      <c r="G62" s="44"/>
-    </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G62" s="44" t="s">
+        <v>7793</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>7606</v>
       </c>
@@ -65762,8 +66144,11 @@
       <c r="F63" s="42" t="s">
         <v>7617</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G63" s="41" t="s">
+        <v>7855</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>7606</v>
       </c>
@@ -65780,10 +66165,13 @@
         <v>8352</v>
       </c>
       <c r="F64" s="43" t="s">
-        <v>7788</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7782</v>
+      </c>
+      <c r="G64" s="41" t="s">
+        <v>7856</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>7613</v>
       </c>
@@ -65796,8 +66184,11 @@
       <c r="F65" s="42" t="s">
         <v>7612</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="41" t="s">
+        <v>7802</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>7611</v>
       </c>
@@ -65810,8 +66201,11 @@
       <c r="F66" s="42" t="s">
         <v>7610</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G66" s="41" t="s">
+        <v>7803</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>7609</v>
       </c>
@@ -65824,8 +66218,11 @@
       <c r="F67" s="42" t="s">
         <v>7608</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G67" s="41" t="s">
+        <v>7804</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>6050</v>
       </c>
@@ -65838,8 +66235,11 @@
       <c r="F68" s="42" t="s">
         <v>7607</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G68" s="41" t="s">
+        <v>7805</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>7606</v>
       </c>
@@ -65851,6 +66251,9 @@
       </c>
       <c r="F69" s="42" t="s">
         <v>7604</v>
+      </c>
+      <c r="G69" s="41" t="s">
+        <v>7806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>